<commit_message>
Added New $/m^2 metric for analysis
</commit_message>
<xml_diff>
--- a/dptos.xlsx
+++ b/dptos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AB84\First-Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCAD3261-74CE-4809-ADD5-023B8172D311}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5C90CF1-7E5E-415D-866F-31FA75F5B24B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{AC42E626-5A29-4158-A6DB-462C3042FB4C}"/>
   </bookViews>
@@ -39,7 +39,7 @@
     <author>AB84</author>
   </authors>
   <commentList>
-    <comment ref="K4" authorId="0" shapeId="0" xr:uid="{B00AF279-5CC0-499B-A8BD-A6AC2DCEFF39}">
+    <comment ref="O4" authorId="0" shapeId="0" xr:uid="{B00AF279-5CC0-499B-A8BD-A6AC2DCEFF39}">
       <text>
         <r>
           <rPr>
@@ -63,12 +63,61 @@
         </r>
       </text>
     </comment>
+    <comment ref="O12" authorId="0" shapeId="0" xr:uid="{131A7DC2-641A-4091-9614-2A330484F9DC}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>AB84:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+extra</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O18" authorId="0" shapeId="0" xr:uid="{38EABF67-CB81-487F-8C84-91A16F8FAF0B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>AB84:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+60
+</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="60">
   <si>
     <t>m^2</t>
   </si>
@@ -158,12 +207,105 @@
   </si>
   <si>
     <t>Estadio Croata</t>
+  </si>
+  <si>
+    <t>Escuela militar (metro)</t>
+  </si>
+  <si>
+    <t>https://www.portalinmobiliario.com/arriendo/departamento/las-condes-metropolitana/5877086-departamento-amoblado-1-dorm-enfrente-el-estadio-espanolcerca-metro-los-militares-uda</t>
+  </si>
+  <si>
+    <t>Wsup</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>Callao</t>
+  </si>
+  <si>
+    <t>https://www.portalinmobiliario.com/MLC-550588773-napoleon-3211-las-condes-chile-_JM</t>
+  </si>
+  <si>
+    <t>Arriendo minimo 6 meses</t>
+  </si>
+  <si>
+    <t>Menciona que el precio es sin muebles pero no dice cuanto es con muebles</t>
+  </si>
+  <si>
+    <t>https://www.portalinmobiliario.com/arriendo/departamento/las-condes-metropolitana/5586110-el-golf-las-condes-uda</t>
+  </si>
+  <si>
+    <t>https://www.portalinmobiliario.com/arriendo/departamento/las-condes-metropolitana/5847410-callao-versalles-uda</t>
+  </si>
+  <si>
+    <t>La Gloria</t>
+  </si>
+  <si>
+    <t>https://www.portalinmobiliario.com/MLC-544689256-departamento-en-arriendo-de-2-dorm-en-las-condes-_JM</t>
+  </si>
+  <si>
+    <t>incluye wifi, minimo 12 meses</t>
+  </si>
+  <si>
+    <t>https://icom.cl/apartments/#lofts</t>
+  </si>
+  <si>
+    <t>Tobalaba tirado pa Vitacura</t>
+  </si>
+  <si>
+    <t>Contrato de 1 año</t>
+  </si>
+  <si>
+    <t>Apoquindo con Las Condes</t>
+  </si>
+  <si>
+    <t>https://www.portalinmobiliario.com/arriendo/departamento/las-condes-metropolitana/5856111-amoblado-carol-urzua-7030-uda</t>
+  </si>
+  <si>
+    <t>Isidora con Vitacura</t>
+  </si>
+  <si>
+    <t>m^2 util</t>
+  </si>
+  <si>
+    <t>m^2 total</t>
+  </si>
+  <si>
+    <t>https://www.portalinmobiliario.com/arriendo/departamento/las-condes-metropolitana/5797786-vitacura-costanera-center-uda</t>
+  </si>
+  <si>
+    <t>Metro Alcantara</t>
+  </si>
+  <si>
+    <t>1 año</t>
+  </si>
+  <si>
+    <t>https://www.portalinmobiliario.com/MLC-550856267-las-torcazas-19-las-condes-chile-_JM</t>
+  </si>
+  <si>
+    <t>$ por m^2</t>
+  </si>
+  <si>
+    <t>~La Gloria</t>
+  </si>
+  <si>
+    <t>$ por m^2 ajustado por estacionamiento</t>
+  </si>
+  <si>
+    <t>https://www.portalinmobiliario.com/arriendo/departamento/las-condes-metropolitana/5842913-metro-manquehue-uda</t>
+  </si>
+  <si>
+    <t>Alcantara con Colon</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="0.0"/>
+  </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -223,10 +365,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -542,391 +687,1125 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A12BAA8B-88EF-4401-83D7-D0D7F7A97F7B}">
-  <dimension ref="B1:M19"/>
+  <dimension ref="B1:Q21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="30.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.1796875" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="14.90625" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.26953125" customWidth="1"/>
-    <col min="9" max="9" width="6.36328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.90625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.90625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="4.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.453125" customWidth="1"/>
+    <col min="3" max="5" width="4.81640625" customWidth="1"/>
+    <col min="6" max="8" width="8.54296875" customWidth="1"/>
+    <col min="9" max="10" width="14.6328125" customWidth="1"/>
+    <col min="11" max="11" width="11.54296875" customWidth="1"/>
+    <col min="12" max="12" width="10.26953125" customWidth="1"/>
+    <col min="13" max="16" width="7" customWidth="1"/>
+    <col min="17" max="17" width="4.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="1" t="s">
+    <row r="1" spans="2:17" ht="43" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="L1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="M1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="N1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="O1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="P1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="Q1" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>13</v>
       </c>
       <c r="C2">
+        <f t="shared" ref="C2:C21" si="0">IF(E2&lt;&gt;"",E2,D2)</f>
         <v>50</v>
       </c>
       <c r="D2">
+        <v>50</v>
+      </c>
+      <c r="F2">
         <v>420</v>
       </c>
-      <c r="E2">
+      <c r="G2">
         <v>80</v>
       </c>
-      <c r="F2">
-        <f>D2+E2</f>
+      <c r="H2">
+        <f>F2+G2</f>
         <v>500</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" s="2">
+        <f>H2/C2</f>
+        <v>10</v>
+      </c>
+      <c r="J2" s="2">
+        <f>IF(O2&lt;&gt;1,(H2+40)/C2,I2)</f>
+        <v>10.8</v>
+      </c>
+      <c r="K2" t="s">
         <v>11</v>
       </c>
-      <c r="H2" t="s">
+      <c r="L2" t="s">
         <v>12</v>
       </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>1</v>
-      </c>
-      <c r="M2" s="2" t="s">
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>15</v>
       </c>
       <c r="C3">
+        <f t="shared" si="0"/>
         <v>60</v>
       </c>
       <c r="D3">
+        <v>60</v>
+      </c>
+      <c r="E3">
+        <v>60</v>
+      </c>
+      <c r="F3">
         <v>420</v>
       </c>
-      <c r="E3">
+      <c r="G3">
         <v>65</v>
       </c>
-      <c r="F3">
-        <f t="shared" ref="F3:F19" si="0">D3+E3</f>
+      <c r="H3">
+        <f t="shared" ref="H3:H21" si="1">F3+G3</f>
         <v>485</v>
       </c>
-      <c r="G3" t="s">
+      <c r="I3" s="2">
+        <f t="shared" ref="I3:I21" si="2">H3/C3</f>
+        <v>8.0833333333333339</v>
+      </c>
+      <c r="J3" s="2">
+        <f t="shared" ref="J3:J21" si="3">IF(O3&lt;&gt;1,(H3+40)/C3,I3)</f>
+        <v>8.0833333333333339</v>
+      </c>
+      <c r="K3" t="s">
         <v>18</v>
       </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-      <c r="J3">
-        <v>1</v>
-      </c>
-      <c r="K3">
-        <v>1</v>
-      </c>
-      <c r="L3">
-        <v>1</v>
-      </c>
-      <c r="M3" s="2" t="s">
+      <c r="L3" t="s">
+        <v>32</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="O3">
+        <v>1</v>
+      </c>
+      <c r="P3">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>20</v>
       </c>
       <c r="C4">
+        <f t="shared" si="0"/>
         <v>36</v>
       </c>
       <c r="D4">
+        <v>36</v>
+      </c>
+      <c r="E4">
+        <v>36</v>
+      </c>
+      <c r="F4">
         <v>380</v>
       </c>
-      <c r="E4">
+      <c r="G4">
         <v>100</v>
       </c>
-      <c r="F4">
-        <f t="shared" si="0"/>
+      <c r="H4">
+        <f t="shared" si="1"/>
         <v>480</v>
       </c>
-      <c r="K4">
-        <v>0.5</v>
-      </c>
-      <c r="M4" s="2" t="s">
+      <c r="I4" s="2">
+        <f t="shared" si="2"/>
+        <v>13.333333333333334</v>
+      </c>
+      <c r="J4" s="2">
+        <f t="shared" si="3"/>
+        <v>14.444444444444445</v>
+      </c>
+      <c r="L4" t="s">
+        <v>32</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+      <c r="N4">
+        <v>1</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>22</v>
       </c>
       <c r="C5">
+        <f t="shared" si="0"/>
         <v>40</v>
       </c>
       <c r="D5">
+        <v>45</v>
+      </c>
+      <c r="E5">
+        <v>40</v>
+      </c>
+      <c r="F5">
         <v>440</v>
       </c>
-      <c r="E5">
+      <c r="G5">
         <v>50</v>
       </c>
-      <c r="F5">
-        <f t="shared" si="0"/>
+      <c r="H5">
+        <f t="shared" si="1"/>
         <v>490</v>
       </c>
-      <c r="I5">
-        <v>1</v>
-      </c>
-      <c r="J5">
-        <v>1</v>
-      </c>
-      <c r="K5">
-        <v>1</v>
-      </c>
-      <c r="L5">
-        <v>1</v>
-      </c>
-      <c r="M5" s="2" t="s">
+      <c r="I5" s="2">
+        <f t="shared" si="2"/>
+        <v>12.25</v>
+      </c>
+      <c r="J5" s="2">
+        <f t="shared" si="3"/>
+        <v>12.25</v>
+      </c>
+      <c r="L5" t="s">
+        <v>32</v>
+      </c>
+      <c r="M5">
+        <v>1</v>
+      </c>
+      <c r="N5">
+        <v>1</v>
+      </c>
+      <c r="O5">
+        <v>1</v>
+      </c>
+      <c r="P5">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>24</v>
       </c>
       <c r="C6">
+        <f t="shared" si="0"/>
         <v>58</v>
       </c>
       <c r="D6">
+        <v>58</v>
+      </c>
+      <c r="E6">
+        <v>58</v>
+      </c>
+      <c r="F6">
         <v>370</v>
       </c>
-      <c r="E6">
+      <c r="G6">
         <v>100</v>
       </c>
-      <c r="F6">
-        <f t="shared" si="0"/>
+      <c r="H6">
+        <f t="shared" si="1"/>
         <v>470</v>
       </c>
-      <c r="I6">
-        <v>1</v>
-      </c>
-      <c r="J6">
-        <v>1</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="L6">
-        <v>0</v>
-      </c>
-      <c r="M6" s="2" t="s">
+      <c r="I6" s="2">
+        <f t="shared" si="2"/>
+        <v>8.1034482758620694</v>
+      </c>
+      <c r="J6" s="2">
+        <f t="shared" si="3"/>
+        <v>8.7931034482758612</v>
+      </c>
+      <c r="L6" t="s">
+        <v>32</v>
+      </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="N6">
+        <v>1</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>27</v>
       </c>
       <c r="C7">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="D7">
         <v>42</v>
       </c>
-      <c r="D7">
+      <c r="E7">
+        <v>40</v>
+      </c>
+      <c r="F7">
         <v>380</v>
       </c>
-      <c r="E7">
-        <f>F7-D7</f>
+      <c r="G7">
+        <f>H7-F7</f>
         <v>110</v>
       </c>
-      <c r="F7">
+      <c r="H7">
         <v>490</v>
       </c>
-      <c r="I7">
-        <v>1</v>
-      </c>
-      <c r="J7">
-        <v>1</v>
-      </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
-      <c r="L7">
-        <v>0</v>
-      </c>
-      <c r="M7" s="2" t="s">
+      <c r="I7" s="2">
+        <f t="shared" si="2"/>
+        <v>12.25</v>
+      </c>
+      <c r="J7" s="2">
+        <f t="shared" si="3"/>
+        <v>13.25</v>
+      </c>
+      <c r="L7" t="s">
+        <v>32</v>
+      </c>
+      <c r="M7">
+        <v>1</v>
+      </c>
+      <c r="N7">
+        <v>1</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>27</v>
       </c>
       <c r="C8">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="D8">
         <v>42</v>
       </c>
-      <c r="D8">
+      <c r="E8">
+        <v>40</v>
+      </c>
+      <c r="F8">
         <v>400</v>
       </c>
-      <c r="E8">
+      <c r="G8">
         <v>135</v>
       </c>
-      <c r="F8">
-        <f t="shared" si="0"/>
+      <c r="H8">
+        <f t="shared" si="1"/>
         <v>535</v>
       </c>
-      <c r="I8">
-        <v>1</v>
-      </c>
-      <c r="J8">
-        <v>1</v>
-      </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
-      <c r="L8">
-        <v>0</v>
-      </c>
-      <c r="M8" s="2" t="s">
+      <c r="I8" s="2">
+        <f t="shared" si="2"/>
+        <v>13.375</v>
+      </c>
+      <c r="J8" s="2">
+        <f t="shared" si="3"/>
+        <v>14.375</v>
+      </c>
+      <c r="L8" t="s">
+        <v>32</v>
+      </c>
+      <c r="M8">
+        <v>1</v>
+      </c>
+      <c r="N8">
+        <v>1</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>29</v>
       </c>
       <c r="C9">
+        <f t="shared" si="0"/>
         <v>60</v>
       </c>
       <c r="D9">
+        <v>60</v>
+      </c>
+      <c r="E9">
+        <v>60</v>
+      </c>
+      <c r="F9">
         <v>450</v>
       </c>
-      <c r="E9">
+      <c r="G9">
         <v>70</v>
       </c>
-      <c r="F9">
+      <c r="H9">
+        <f t="shared" si="1"/>
+        <v>520</v>
+      </c>
+      <c r="I9" s="2">
+        <f t="shared" si="2"/>
+        <v>8.6666666666666661</v>
+      </c>
+      <c r="J9" s="2">
+        <f t="shared" si="3"/>
+        <v>9.3333333333333339</v>
+      </c>
+      <c r="L9" t="s">
+        <v>32</v>
+      </c>
+      <c r="M9">
+        <v>2</v>
+      </c>
+      <c r="N9">
+        <v>2</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10">
         <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="D10">
+        <v>51</v>
+      </c>
+      <c r="E10">
+        <v>47</v>
+      </c>
+      <c r="F10">
+        <v>420</v>
+      </c>
+      <c r="G10">
+        <v>58</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="1"/>
+        <v>478</v>
+      </c>
+      <c r="I10" s="2">
+        <f t="shared" si="2"/>
+        <v>10.170212765957446</v>
+      </c>
+      <c r="J10" s="2">
+        <f t="shared" si="3"/>
+        <v>10.170212765957446</v>
+      </c>
+      <c r="L10" t="s">
+        <v>32</v>
+      </c>
+      <c r="M10">
+        <v>1</v>
+      </c>
+      <c r="N10">
+        <v>1</v>
+      </c>
+      <c r="O10">
+        <v>1</v>
+      </c>
+      <c r="P10">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11">
+        <v>55</v>
+      </c>
+      <c r="F11">
+        <v>420</v>
+      </c>
+      <c r="G11">
+        <v>100</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="1"/>
         <v>520</v>
       </c>
-      <c r="I9">
+      <c r="I11" s="2">
+        <f t="shared" si="2"/>
+        <v>9.454545454545455</v>
+      </c>
+      <c r="J11" s="2">
+        <f t="shared" si="3"/>
+        <v>9.454545454545455</v>
+      </c>
+      <c r="L11" t="s">
+        <v>32</v>
+      </c>
+      <c r="M11">
+        <v>1</v>
+      </c>
+      <c r="N11">
+        <v>1</v>
+      </c>
+      <c r="O11">
+        <v>1</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="D12">
+        <v>55</v>
+      </c>
+      <c r="E12">
+        <v>49</v>
+      </c>
+      <c r="F12">
+        <v>450</v>
+      </c>
+      <c r="G12">
+        <v>120</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="1"/>
+        <v>570</v>
+      </c>
+      <c r="I12" s="2">
+        <f t="shared" si="2"/>
+        <v>11.63265306122449</v>
+      </c>
+      <c r="J12" s="2">
+        <f t="shared" si="3"/>
+        <v>12.448979591836734</v>
+      </c>
+      <c r="L12" t="s">
+        <v>33</v>
+      </c>
+      <c r="M12">
+        <v>1</v>
+      </c>
+      <c r="N12">
+        <v>1</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="D13">
+        <v>65</v>
+      </c>
+      <c r="E13">
+        <v>60</v>
+      </c>
+      <c r="F13">
+        <v>450</v>
+      </c>
+      <c r="G13">
+        <v>60</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="1"/>
+        <v>510</v>
+      </c>
+      <c r="I13" s="2">
+        <f t="shared" si="2"/>
+        <v>8.5</v>
+      </c>
+      <c r="J13" s="2">
+        <f t="shared" si="3"/>
+        <v>9.1666666666666661</v>
+      </c>
+      <c r="K13" t="s">
+        <v>36</v>
+      </c>
+      <c r="L13" t="s">
+        <v>33</v>
+      </c>
+      <c r="M13">
+        <v>1</v>
+      </c>
+      <c r="N13">
+        <v>1</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="D14">
+        <v>46</v>
+      </c>
+      <c r="E14">
+        <v>40</v>
+      </c>
+      <c r="F14">
+        <v>400</v>
+      </c>
+      <c r="G14">
+        <v>50</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="1"/>
+        <v>450</v>
+      </c>
+      <c r="I14" s="2">
+        <f t="shared" si="2"/>
+        <v>11.25</v>
+      </c>
+      <c r="J14" s="2">
+        <f t="shared" si="3"/>
+        <v>11.25</v>
+      </c>
+      <c r="K14" t="s">
+        <v>37</v>
+      </c>
+      <c r="L14" t="s">
+        <v>33</v>
+      </c>
+      <c r="M14">
+        <v>1</v>
+      </c>
+      <c r="N14">
+        <v>1</v>
+      </c>
+      <c r="O14">
+        <v>1</v>
+      </c>
+      <c r="P14">
+        <v>1</v>
+      </c>
+      <c r="Q14" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>61</v>
+      </c>
+      <c r="D15">
+        <v>64</v>
+      </c>
+      <c r="E15">
+        <v>61</v>
+      </c>
+      <c r="F15">
+        <v>450</v>
+      </c>
+      <c r="G15">
+        <v>100</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="1"/>
+        <v>550</v>
+      </c>
+      <c r="I15" s="2">
+        <f t="shared" si="2"/>
+        <v>9.0163934426229506</v>
+      </c>
+      <c r="J15" s="2">
+        <f t="shared" si="3"/>
+        <v>9.0163934426229506</v>
+      </c>
+      <c r="L15" t="s">
+        <v>33</v>
+      </c>
+      <c r="M15">
         <v>2</v>
       </c>
-      <c r="J9">
+      <c r="N15">
         <v>2</v>
       </c>
-      <c r="M9" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="F10">
+      <c r="O15">
+        <v>1</v>
+      </c>
+      <c r="P15">
+        <v>1</v>
+      </c>
+      <c r="Q15" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B16" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="F11">
+        <v>42</v>
+      </c>
+      <c r="E16">
+        <v>42</v>
+      </c>
+      <c r="F16">
+        <v>435</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="1"/>
+        <v>435</v>
+      </c>
+      <c r="I16" s="2">
+        <f t="shared" si="2"/>
+        <v>10.357142857142858</v>
+      </c>
+      <c r="J16" s="2">
+        <f t="shared" si="3"/>
+        <v>11.30952380952381</v>
+      </c>
+      <c r="K16" t="s">
+        <v>42</v>
+      </c>
+      <c r="L16" t="s">
+        <v>33</v>
+      </c>
+      <c r="M16">
+        <v>1</v>
+      </c>
+      <c r="N16">
+        <v>1</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
+      <c r="P16">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B17" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="F12">
+        <v>46</v>
+      </c>
+      <c r="D17">
+        <v>52</v>
+      </c>
+      <c r="E17">
+        <v>46</v>
+      </c>
+      <c r="F17">
+        <v>450</v>
+      </c>
+      <c r="G17">
+        <v>50</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="1"/>
+        <v>500</v>
+      </c>
+      <c r="I17" s="2">
+        <f t="shared" si="2"/>
+        <v>10.869565217391305</v>
+      </c>
+      <c r="J17" s="2">
+        <f t="shared" si="3"/>
+        <v>10.869565217391305</v>
+      </c>
+      <c r="K17" t="s">
+        <v>45</v>
+      </c>
+      <c r="L17" t="s">
+        <v>33</v>
+      </c>
+      <c r="M17">
+        <v>1</v>
+      </c>
+      <c r="N17">
+        <v>1</v>
+      </c>
+      <c r="O17">
+        <v>1</v>
+      </c>
+      <c r="P17">
+        <v>1</v>
+      </c>
+      <c r="Q17" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B18" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="F13">
+        <v>40</v>
+      </c>
+      <c r="D18">
+        <v>45</v>
+      </c>
+      <c r="E18">
+        <v>40</v>
+      </c>
+      <c r="F18">
+        <v>420</v>
+      </c>
+      <c r="G18">
+        <v>68</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="1"/>
+        <v>488</v>
+      </c>
+      <c r="I18" s="2">
+        <f t="shared" si="2"/>
+        <v>12.2</v>
+      </c>
+      <c r="J18" s="2">
+        <f t="shared" si="3"/>
+        <v>13.2</v>
+      </c>
+      <c r="L18" t="s">
+        <v>33</v>
+      </c>
+      <c r="M18">
+        <v>1</v>
+      </c>
+      <c r="N18">
+        <v>1</v>
+      </c>
+      <c r="O18">
+        <v>0</v>
+      </c>
+      <c r="P18">
+        <v>1</v>
+      </c>
+      <c r="Q18" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B19" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="F14">
+        <v>45</v>
+      </c>
+      <c r="D19">
+        <v>50</v>
+      </c>
+      <c r="E19">
+        <v>45</v>
+      </c>
+      <c r="F19">
+        <v>400</v>
+      </c>
+      <c r="G19">
+        <v>120</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="1"/>
+        <v>520</v>
+      </c>
+      <c r="I19" s="2">
+        <f t="shared" si="2"/>
+        <v>11.555555555555555</v>
+      </c>
+      <c r="J19" s="2">
+        <f t="shared" si="3"/>
+        <v>12.444444444444445</v>
+      </c>
+      <c r="K19" t="s">
+        <v>53</v>
+      </c>
+      <c r="L19" t="s">
+        <v>33</v>
+      </c>
+      <c r="M19">
+        <v>1</v>
+      </c>
+      <c r="N19">
+        <v>1</v>
+      </c>
+      <c r="O19">
+        <v>0</v>
+      </c>
+      <c r="P19">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B20" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="F15">
+        <v>43</v>
+      </c>
+      <c r="D20">
+        <v>48</v>
+      </c>
+      <c r="E20">
+        <v>43</v>
+      </c>
+      <c r="F20">
+        <v>420</v>
+      </c>
+      <c r="G20">
+        <v>75</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="1"/>
+        <v>495</v>
+      </c>
+      <c r="I20" s="2">
+        <f t="shared" si="2"/>
+        <v>11.511627906976743</v>
+      </c>
+      <c r="J20" s="2">
+        <f t="shared" si="3"/>
+        <v>11.511627906976743</v>
+      </c>
+      <c r="L20" t="s">
+        <v>33</v>
+      </c>
+      <c r="M20">
+        <v>1</v>
+      </c>
+      <c r="N20">
+        <v>1</v>
+      </c>
+      <c r="O20">
+        <v>1</v>
+      </c>
+      <c r="P20">
+        <v>1</v>
+      </c>
+      <c r="Q20" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B21" t="s">
+        <v>59</v>
+      </c>
+      <c r="C21">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="F16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="6:6" x14ac:dyDescent="0.35">
-      <c r="F17">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="6:6" x14ac:dyDescent="0.35">
-      <c r="F18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="6:6" x14ac:dyDescent="0.35">
-      <c r="F19">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>50</v>
+      </c>
+      <c r="D21">
+        <v>50</v>
+      </c>
+      <c r="E21">
+        <v>50</v>
+      </c>
+      <c r="F21">
+        <v>360</v>
+      </c>
+      <c r="G21">
+        <v>80</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="1"/>
+        <v>440</v>
+      </c>
+      <c r="I21" s="2">
+        <f t="shared" si="2"/>
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="J21" s="2">
+        <f t="shared" si="3"/>
+        <v>9.6</v>
+      </c>
+      <c r="L21" t="s">
+        <v>33</v>
+      </c>
+      <c r="M21">
+        <v>1</v>
+      </c>
+      <c r="N21">
+        <v>1</v>
+      </c>
+      <c r="O21">
+        <v>0</v>
+      </c>
+      <c r="P21">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="J2:J21">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="M2" r:id="rId1" xr:uid="{BC09F7C9-7B72-4359-95B0-C2E1E05EF957}"/>
-    <hyperlink ref="M3" r:id="rId2" xr:uid="{F038CDB1-8A86-4688-A6D6-EFF4B88ACBC9}"/>
-    <hyperlink ref="M4" r:id="rId3" xr:uid="{DA72C175-A4E0-46ED-9774-B5F9A8BBBAE0}"/>
-    <hyperlink ref="M5" r:id="rId4" xr:uid="{FE2AA06A-6A35-4937-BE49-B7B45B21F0D5}"/>
-    <hyperlink ref="M6" r:id="rId5" xr:uid="{2E4012BE-EB79-4012-A169-A991ACE7F117}"/>
-    <hyperlink ref="M7" r:id="rId6" xr:uid="{A02D9B5E-53BF-4A4A-BDC2-FE594C51D634}"/>
-    <hyperlink ref="M8" r:id="rId7" xr:uid="{8FA9A79E-6898-4660-9DE9-6F7EFEA61F05}"/>
-    <hyperlink ref="M9" r:id="rId8" xr:uid="{B88818F4-85EA-4C04-A015-0ECD67F9BC0C}"/>
+    <hyperlink ref="Q2" r:id="rId1" xr:uid="{BC09F7C9-7B72-4359-95B0-C2E1E05EF957}"/>
+    <hyperlink ref="Q3" r:id="rId2" xr:uid="{F038CDB1-8A86-4688-A6D6-EFF4B88ACBC9}"/>
+    <hyperlink ref="Q4" r:id="rId3" xr:uid="{DA72C175-A4E0-46ED-9774-B5F9A8BBBAE0}"/>
+    <hyperlink ref="Q5" r:id="rId4" xr:uid="{FE2AA06A-6A35-4937-BE49-B7B45B21F0D5}"/>
+    <hyperlink ref="Q6" r:id="rId5" xr:uid="{2E4012BE-EB79-4012-A169-A991ACE7F117}"/>
+    <hyperlink ref="Q7" r:id="rId6" xr:uid="{A02D9B5E-53BF-4A4A-BDC2-FE594C51D634}"/>
+    <hyperlink ref="Q8" r:id="rId7" xr:uid="{8FA9A79E-6898-4660-9DE9-6F7EFEA61F05}"/>
+    <hyperlink ref="Q9" r:id="rId8" xr:uid="{B88818F4-85EA-4C04-A015-0ECD67F9BC0C}"/>
+    <hyperlink ref="Q10" r:id="rId9" xr:uid="{12FE4701-FD57-4DEE-A050-02AA65B15321}"/>
+    <hyperlink ref="Q12" r:id="rId10" xr:uid="{8D75F53D-2337-467A-B53E-FC3A975384F5}"/>
+    <hyperlink ref="Q14" r:id="rId11" xr:uid="{E55BA592-81C1-4CFF-B914-814C72CD5900}"/>
+    <hyperlink ref="Q13" r:id="rId12" xr:uid="{CC2D0F41-FC4B-4FBE-BA19-4A2F07D1C48B}"/>
+    <hyperlink ref="Q15" r:id="rId13" xr:uid="{F01F7903-CB22-4162-976E-157168585DF5}"/>
+    <hyperlink ref="Q16" r:id="rId14" location="lofts" xr:uid="{7C02D451-FEA2-4D9B-A8CC-2BB27509D8FF}"/>
+    <hyperlink ref="Q17" r:id="rId15" xr:uid="{D8C6B8A0-C8A3-4B20-82FD-064CF0E61167}"/>
+    <hyperlink ref="Q18" r:id="rId16" xr:uid="{C8851664-C1E9-4EFC-B52A-BDC05728D40F}"/>
+    <hyperlink ref="Q19" r:id="rId17" xr:uid="{D5C3517C-A7D7-4944-8840-1CF35728AA10}"/>
+    <hyperlink ref="Q20" r:id="rId18" xr:uid="{8F083F3D-C61C-4983-BE1E-3B788A7C8D12}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId9"/>
-  <legacyDrawing r:id="rId10"/>
+  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId19"/>
+  <legacyDrawing r:id="rId20"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
-Added more entries with new incoming data -Added color coding to price column
</commit_message>
<xml_diff>
--- a/dptos.xlsx
+++ b/dptos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AB84\First-Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F0BA1E8-212A-4DEA-8F2B-1911AF2D15F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4538A95B-AA1F-43E1-BFE4-5A02B194CF16}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{AC42E626-5A29-4158-A6DB-462C3042FB4C}"/>
   </bookViews>
@@ -39,7 +39,7 @@
     <author>AB84</author>
   </authors>
   <commentList>
-    <comment ref="O4" authorId="0" shapeId="0" xr:uid="{B00AF279-5CC0-499B-A8BD-A6AC2DCEFF39}">
+    <comment ref="N4" authorId="0" shapeId="0" xr:uid="{B00AF279-5CC0-499B-A8BD-A6AC2DCEFF39}">
       <text>
         <r>
           <rPr>
@@ -63,7 +63,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O12" authorId="0" shapeId="0" xr:uid="{131A7DC2-641A-4091-9614-2A330484F9DC}">
+    <comment ref="N12" authorId="0" shapeId="0" xr:uid="{131A7DC2-641A-4091-9614-2A330484F9DC}">
       <text>
         <r>
           <rPr>
@@ -87,7 +87,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O18" authorId="0" shapeId="0" xr:uid="{38EABF67-CB81-487F-8C84-91A16F8FAF0B}">
+    <comment ref="N18" authorId="0" shapeId="0" xr:uid="{38EABF67-CB81-487F-8C84-91A16F8FAF0B}">
       <text>
         <r>
           <rPr>
@@ -112,12 +112,60 @@
         </r>
       </text>
     </comment>
+    <comment ref="N24" authorId="0" shapeId="0" xr:uid="{FA75EAF1-0497-4167-9615-E143ED96933F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>AB84:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+75</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N26" authorId="0" shapeId="0" xr:uid="{8BA8CD98-6942-4CF8-B15E-9A3A983CBAC2}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>AB84:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+50</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="76">
   <si>
     <t>m^2</t>
   </si>
@@ -297,6 +345,54 @@
   </si>
   <si>
     <t>Alcantara con Colon</t>
+  </si>
+  <si>
+    <t>Los Leones</t>
+  </si>
+  <si>
+    <t>Da Vinci</t>
+  </si>
+  <si>
+    <t>https://www.portalinmobiliario.com/MLC-545543913-departamento-en-arriendo-de-1-dorm-en-providencia-_JM#reco_item_pos=14&amp;reco_backend=user_navigation&amp;reco_backend_type=function&amp;reco_client=classi_portalinmobiliario_navigation&amp;reco_id=ae77e213-7c53-4a83-8240-0ef49e221d10&amp;page=navigation</t>
+  </si>
+  <si>
+    <t>https://www.portalinmobiliario.com/arriendo/departamento/las-condes-metropolitana/5872440-amoblado-leonardo-da-vinci-7500-uda</t>
+  </si>
+  <si>
+    <t>https://www.portalinmobiliario.com/arriendo/departamento/las-condes-metropolitana/5876850-metro-el-golf-amoblado-encomendero-200-uda</t>
+  </si>
+  <si>
+    <t>https://www.portalinmobiliario.com/arriendo/departamento/las-condes-metropolitana/5881970-la-gloria-apoquindo-metro-uda</t>
+  </si>
+  <si>
+    <t>Manquehue sur</t>
+  </si>
+  <si>
+    <t>https://www.portalinmobiliario.com/arriendo/departamento/las-condes-metropolitana/5703357-luis-zegers-apoquindo-uda</t>
+  </si>
+  <si>
+    <t>Wsup 2399</t>
+  </si>
+  <si>
+    <t>Wsup 0545</t>
+  </si>
+  <si>
+    <t>https://www.portalinmobiliario.com/arriendo/departamento/las-condes-metropolitana/5758450-metro-escuela-militar-uda</t>
+  </si>
+  <si>
+    <t>https://www.portalinmobiliario.com/MLC-550413742-alcantara-970-las-condes-chile-_JM</t>
+  </si>
+  <si>
+    <t>Arriendo sube 120 en Enero</t>
+  </si>
+  <si>
+    <t>Fancy Moden Look</t>
+  </si>
+  <si>
+    <t>Parece Hotel</t>
+  </si>
+  <si>
+    <t>Looks Reallly Good</t>
   </si>
 </sst>
 </file>
@@ -365,13 +461,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -687,519 +784,535 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A12BAA8B-88EF-4401-83D7-D0D7F7A97F7B}">
-  <dimension ref="B1:Q21"/>
+  <dimension ref="A1:R27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="23.453125" customWidth="1"/>
-    <col min="3" max="5" width="4.81640625" customWidth="1"/>
-    <col min="6" max="8" width="8.54296875" customWidth="1"/>
-    <col min="9" max="10" width="14.6328125" customWidth="1"/>
-    <col min="11" max="11" width="11.54296875" customWidth="1"/>
-    <col min="12" max="12" width="10.26953125" customWidth="1"/>
-    <col min="13" max="16" width="7" customWidth="1"/>
-    <col min="17" max="17" width="4.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.453125" customWidth="1"/>
+    <col min="2" max="3" width="7" customWidth="1"/>
+    <col min="4" max="6" width="4.81640625" customWidth="1"/>
+    <col min="7" max="9" width="8.54296875" customWidth="1"/>
+    <col min="10" max="11" width="14.6328125" customWidth="1"/>
+    <col min="12" max="12" width="11.54296875" customWidth="1"/>
+    <col min="13" max="13" width="10.26953125" customWidth="1"/>
+    <col min="14" max="17" width="7" customWidth="1"/>
+    <col min="18" max="18" width="4.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:17" ht="43" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" ht="43" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>1</v>
+      </c>
       <c r="B1" s="3" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="3" t="s">
-        <v>17</v>
-      </c>
       <c r="N1" s="3" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="P1" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <f t="shared" ref="D2:D27" si="0">IF(F2&lt;&gt;"",F2,E2)</f>
+        <v>50</v>
+      </c>
+      <c r="E2">
+        <v>50</v>
+      </c>
+      <c r="G2">
+        <v>420</v>
+      </c>
+      <c r="H2">
+        <v>80</v>
+      </c>
+      <c r="I2">
+        <f>G2+H2</f>
+        <v>500</v>
+      </c>
+      <c r="J2" s="2">
+        <f>I2/D2</f>
         <v>10</v>
       </c>
-      <c r="Q1" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2">
-        <f t="shared" ref="C2:C21" si="0">IF(E2&lt;&gt;"",E2,D2)</f>
-        <v>50</v>
-      </c>
-      <c r="D2">
-        <v>50</v>
-      </c>
-      <c r="F2">
-        <v>420</v>
-      </c>
-      <c r="G2">
-        <v>80</v>
-      </c>
-      <c r="H2">
-        <f>F2+G2</f>
-        <v>500</v>
-      </c>
-      <c r="I2" s="2">
-        <f>H2/C2</f>
-        <v>10</v>
-      </c>
-      <c r="J2" s="2">
-        <f>IF(O2&lt;&gt;1,(H2+40)/C2,I2)</f>
-        <v>10.8</v>
-      </c>
-      <c r="K2" t="s">
+      <c r="K2" s="2">
+        <f>IF(N2&lt;&gt;1,(I2+50)/D2,J2)</f>
         <v>11</v>
       </c>
       <c r="L2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M2" t="s">
         <v>12</v>
       </c>
-      <c r="M2">
-        <v>1</v>
-      </c>
       <c r="N2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O2">
-        <v>0</v>
-      </c>
-      <c r="P2">
-        <v>1</v>
-      </c>
-      <c r="Q2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="R2" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B3" t="s">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
         <v>15</v>
       </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
       <c r="C3">
-        <f t="shared" si="0"/>
-        <v>60</v>
+        <v>1</v>
       </c>
       <c r="D3">
+        <f t="shared" si="0"/>
         <v>60</v>
       </c>
       <c r="E3">
         <v>60</v>
       </c>
       <c r="F3">
+        <v>60</v>
+      </c>
+      <c r="G3">
         <v>420</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>65</v>
       </c>
-      <c r="H3">
-        <f t="shared" ref="H3:H21" si="1">F3+G3</f>
+      <c r="I3">
+        <f t="shared" ref="I3:I27" si="1">G3+H3</f>
         <v>485</v>
       </c>
-      <c r="I3" s="2">
-        <f t="shared" ref="I3:I21" si="2">H3/C3</f>
+      <c r="J3" s="2">
+        <f t="shared" ref="J3:J27" si="2">I3/D3</f>
         <v>8.0833333333333339</v>
       </c>
-      <c r="J3" s="2">
-        <f t="shared" ref="J3:J21" si="3">IF(O3&lt;&gt;1,(H3+40)/C3,I3)</f>
+      <c r="K3" s="2">
+        <f t="shared" ref="K3:K27" si="3">IF(N3&lt;&gt;1,(I3+50)/D3,J3)</f>
         <v>8.0833333333333339</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>18</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>32</v>
       </c>
-      <c r="M3">
-        <v>1</v>
-      </c>
       <c r="N3">
         <v>1</v>
       </c>
       <c r="O3">
         <v>1</v>
       </c>
-      <c r="P3">
-        <v>1</v>
-      </c>
-      <c r="Q3" s="1" t="s">
+      <c r="R3" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B4" t="s">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A4" s="4" t="s">
         <v>20</v>
       </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
       <c r="C4">
-        <f t="shared" si="0"/>
-        <v>36</v>
+        <v>1</v>
       </c>
       <c r="D4">
+        <f t="shared" si="0"/>
         <v>36</v>
       </c>
       <c r="E4">
         <v>36</v>
       </c>
       <c r="F4">
+        <v>36</v>
+      </c>
+      <c r="G4">
         <v>380</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>100</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <f t="shared" si="1"/>
         <v>480</v>
       </c>
-      <c r="I4" s="2">
+      <c r="J4" s="2">
         <f t="shared" si="2"/>
         <v>13.333333333333334</v>
       </c>
-      <c r="J4" s="2">
-        <f t="shared" si="3"/>
-        <v>14.444444444444445</v>
-      </c>
-      <c r="L4" t="s">
+      <c r="K4" s="2">
+        <f t="shared" si="3"/>
+        <v>14.722222222222221</v>
+      </c>
+      <c r="M4" t="s">
         <v>32</v>
       </c>
-      <c r="M4">
-        <v>1</v>
-      </c>
       <c r="N4">
-        <v>1</v>
-      </c>
-      <c r="O4">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R4" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B5" t="s">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A5" s="4" t="s">
         <v>22</v>
       </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
       <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>45</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>40</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>440</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>50</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <f t="shared" si="1"/>
         <v>490</v>
       </c>
-      <c r="I5" s="2">
+      <c r="J5" s="2">
         <f t="shared" si="2"/>
         <v>12.25</v>
       </c>
-      <c r="J5" s="2">
+      <c r="K5" s="2">
         <f t="shared" si="3"/>
         <v>12.25</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>32</v>
       </c>
-      <c r="M5">
-        <v>1</v>
-      </c>
       <c r="N5">
         <v>1</v>
       </c>
       <c r="O5">
         <v>1</v>
       </c>
-      <c r="P5">
-        <v>1</v>
-      </c>
-      <c r="Q5" s="1" t="s">
+      <c r="R5" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B6" t="s">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A6" s="4" t="s">
         <v>24</v>
       </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
       <c r="C6">
-        <f t="shared" si="0"/>
-        <v>58</v>
+        <v>1</v>
       </c>
       <c r="D6">
+        <f t="shared" si="0"/>
         <v>58</v>
       </c>
       <c r="E6">
         <v>58</v>
       </c>
       <c r="F6">
+        <v>58</v>
+      </c>
+      <c r="G6">
         <v>370</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>100</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <f t="shared" si="1"/>
         <v>470</v>
       </c>
-      <c r="I6" s="2">
+      <c r="J6" s="2">
         <f t="shared" si="2"/>
         <v>8.1034482758620694</v>
       </c>
-      <c r="J6" s="2">
-        <f t="shared" si="3"/>
-        <v>8.7931034482758612</v>
-      </c>
-      <c r="L6" t="s">
+      <c r="K6" s="2">
+        <f t="shared" si="3"/>
+        <v>8.9655172413793096</v>
+      </c>
+      <c r="M6" t="s">
         <v>32</v>
       </c>
-      <c r="M6">
-        <v>1</v>
-      </c>
       <c r="N6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O6">
         <v>0</v>
       </c>
-      <c r="P6">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="1" t="s">
+      <c r="Q6">
+        <v>1</v>
+      </c>
+      <c r="R6" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B7" t="s">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A7" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
       <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>42</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>40</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>380</v>
       </c>
-      <c r="G7">
-        <f>H7-F7</f>
+      <c r="H7">
+        <f>I7-G7</f>
         <v>110</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>490</v>
       </c>
-      <c r="I7" s="2">
+      <c r="J7" s="2">
         <f t="shared" si="2"/>
         <v>12.25</v>
       </c>
-      <c r="J7" s="2">
-        <f t="shared" si="3"/>
-        <v>13.25</v>
-      </c>
-      <c r="L7" t="s">
+      <c r="K7" s="2">
+        <f t="shared" si="3"/>
+        <v>13.5</v>
+      </c>
+      <c r="M7" t="s">
         <v>32</v>
       </c>
-      <c r="M7">
-        <v>1</v>
-      </c>
       <c r="N7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O7">
         <v>0</v>
       </c>
-      <c r="P7">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="1" t="s">
+      <c r="R7" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B8" t="s">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A8" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
       <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>42</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>40</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>400</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>135</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <f t="shared" si="1"/>
         <v>535</v>
       </c>
-      <c r="I8" s="2">
+      <c r="J8" s="2">
         <f t="shared" si="2"/>
         <v>13.375</v>
       </c>
-      <c r="J8" s="2">
-        <f t="shared" si="3"/>
-        <v>14.375</v>
-      </c>
-      <c r="L8" t="s">
+      <c r="K8" s="2">
+        <f t="shared" si="3"/>
+        <v>14.625</v>
+      </c>
+      <c r="M8" t="s">
         <v>32</v>
       </c>
-      <c r="M8">
-        <v>1</v>
-      </c>
       <c r="N8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O8">
         <v>0</v>
       </c>
-      <c r="P8">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="1" t="s">
+      <c r="R8" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B9" t="s">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A9" s="4" t="s">
         <v>29</v>
       </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
       <c r="C9">
-        <f t="shared" si="0"/>
-        <v>60</v>
+        <v>2</v>
       </c>
       <c r="D9">
+        <f t="shared" si="0"/>
         <v>60</v>
       </c>
       <c r="E9">
         <v>60</v>
       </c>
       <c r="F9">
+        <v>60</v>
+      </c>
+      <c r="G9">
         <v>450</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>70</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <f t="shared" si="1"/>
         <v>520</v>
       </c>
-      <c r="I9" s="2">
+      <c r="J9" s="2">
         <f t="shared" si="2"/>
         <v>8.6666666666666661</v>
       </c>
-      <c r="J9" s="2">
-        <f t="shared" si="3"/>
-        <v>9.3333333333333339</v>
-      </c>
-      <c r="L9" t="s">
+      <c r="K9" s="2">
+        <f t="shared" si="3"/>
+        <v>9.5</v>
+      </c>
+      <c r="M9" t="s">
         <v>32</v>
       </c>
-      <c r="M9">
-        <v>2</v>
-      </c>
       <c r="N9">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O9">
         <v>0</v>
       </c>
-      <c r="P9">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="1" t="s">
+      <c r="R9" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B10" t="s">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A10" s="4" t="s">
         <v>30</v>
       </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
       <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
         <f t="shared" si="0"/>
         <v>47</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>51</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>47</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>420</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>58</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <f t="shared" si="1"/>
         <v>478</v>
       </c>
-      <c r="I10" s="2">
+      <c r="J10" s="2">
         <f t="shared" si="2"/>
         <v>10.170212765957446</v>
       </c>
-      <c r="J10" s="2">
+      <c r="K10" s="2">
         <f t="shared" si="3"/>
         <v>10.170212765957446</v>
       </c>
-      <c r="L10" t="s">
-        <v>32</v>
-      </c>
-      <c r="M10">
-        <v>1</v>
+      <c r="M10" t="s">
+        <v>68</v>
       </c>
       <c r="N10">
         <v>1</v>
@@ -1207,353 +1320,369 @@
       <c r="O10">
         <v>1</v>
       </c>
-      <c r="P10">
-        <v>1</v>
-      </c>
-      <c r="Q10" s="1" t="s">
+      <c r="R10" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B11" t="s">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A11" s="4" t="s">
         <v>30</v>
       </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
       <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
         <v>55</v>
       </c>
+      <c r="E11">
+        <v>55</v>
+      </c>
       <c r="F11">
+        <v>55</v>
+      </c>
+      <c r="G11">
         <v>420</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>100</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <f t="shared" si="1"/>
         <v>520</v>
       </c>
-      <c r="I11" s="2">
+      <c r="J11" s="2">
         <f t="shared" si="2"/>
         <v>9.454545454545455</v>
       </c>
-      <c r="J11" s="2">
+      <c r="K11" s="2">
         <f t="shared" si="3"/>
         <v>9.454545454545455</v>
       </c>
-      <c r="L11" t="s">
-        <v>32</v>
-      </c>
-      <c r="M11">
-        <v>1</v>
+      <c r="M11" t="s">
+        <v>69</v>
       </c>
       <c r="N11">
         <v>1</v>
       </c>
       <c r="O11">
-        <v>1</v>
-      </c>
-      <c r="P11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B12" t="s">
+        <v>0</v>
+      </c>
+      <c r="R11" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A12" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
       <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>55</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>49</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>450</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>120</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <f t="shared" si="1"/>
         <v>570</v>
       </c>
-      <c r="I12" s="2">
+      <c r="J12" s="2">
         <f t="shared" si="2"/>
         <v>11.63265306122449</v>
       </c>
-      <c r="J12" s="2">
-        <f t="shared" si="3"/>
-        <v>12.448979591836734</v>
-      </c>
-      <c r="L12" t="s">
+      <c r="K12" s="2">
+        <f t="shared" si="3"/>
+        <v>12.653061224489797</v>
+      </c>
+      <c r="M12" t="s">
         <v>33</v>
       </c>
-      <c r="M12">
-        <v>1</v>
-      </c>
       <c r="N12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O12">
-        <v>0</v>
-      </c>
-      <c r="P12">
-        <v>1</v>
-      </c>
-      <c r="Q12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="R12" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B13" t="s">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A13" s="4" t="s">
         <v>34</v>
       </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
       <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="D13">
+      <c r="E13">
         <v>65</v>
       </c>
-      <c r="E13">
+      <c r="F13">
         <v>60</v>
       </c>
-      <c r="F13">
+      <c r="G13">
         <v>450</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <v>60</v>
       </c>
-      <c r="H13">
+      <c r="I13">
         <f t="shared" si="1"/>
         <v>510</v>
       </c>
-      <c r="I13" s="2">
+      <c r="J13" s="2">
         <f t="shared" si="2"/>
         <v>8.5</v>
       </c>
-      <c r="J13" s="2">
-        <f t="shared" si="3"/>
-        <v>9.1666666666666661</v>
-      </c>
-      <c r="K13" t="s">
+      <c r="K13" s="2">
+        <f t="shared" si="3"/>
+        <v>9.3333333333333339</v>
+      </c>
+      <c r="L13" t="s">
         <v>36</v>
       </c>
-      <c r="L13" t="s">
+      <c r="M13" t="s">
         <v>33</v>
       </c>
-      <c r="M13">
-        <v>1</v>
-      </c>
       <c r="N13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O13">
         <v>0</v>
       </c>
-      <c r="P13">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="1" t="s">
+      <c r="R13" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B14" t="s">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A14" s="4" t="s">
         <v>22</v>
       </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
       <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="D14">
+      <c r="E14">
         <v>46</v>
       </c>
-      <c r="E14">
+      <c r="F14">
         <v>40</v>
       </c>
-      <c r="F14">
+      <c r="G14">
         <v>400</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <v>50</v>
       </c>
-      <c r="H14">
+      <c r="I14">
         <f t="shared" si="1"/>
         <v>450</v>
       </c>
-      <c r="I14" s="2">
+      <c r="J14" s="2">
         <f t="shared" si="2"/>
         <v>11.25</v>
       </c>
-      <c r="J14" s="2">
+      <c r="K14" s="2">
         <f t="shared" si="3"/>
         <v>11.25</v>
       </c>
-      <c r="K14" t="s">
+      <c r="L14" t="s">
         <v>37</v>
       </c>
-      <c r="L14" t="s">
+      <c r="M14" t="s">
         <v>33</v>
       </c>
-      <c r="M14">
-        <v>1</v>
-      </c>
       <c r="N14">
         <v>1</v>
       </c>
       <c r="O14">
         <v>1</v>
       </c>
-      <c r="P14">
-        <v>1</v>
-      </c>
-      <c r="Q14" s="1" t="s">
+      <c r="R14" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B15" t="s">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A15" s="4" t="s">
         <v>40</v>
       </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
       <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="D15">
         <f t="shared" si="0"/>
         <v>61</v>
       </c>
-      <c r="D15">
+      <c r="E15">
         <v>64</v>
       </c>
-      <c r="E15">
+      <c r="F15">
         <v>61</v>
       </c>
-      <c r="F15">
+      <c r="G15">
         <v>450</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <v>100</v>
       </c>
-      <c r="H15">
+      <c r="I15">
         <f t="shared" si="1"/>
         <v>550</v>
       </c>
-      <c r="I15" s="2">
+      <c r="J15" s="2">
         <f t="shared" si="2"/>
         <v>9.0163934426229506</v>
       </c>
-      <c r="J15" s="2">
-        <f t="shared" si="3"/>
-        <v>9.0163934426229506</v>
+      <c r="K15" s="2">
+        <f t="shared" si="3"/>
+        <v>9.8360655737704921</v>
       </c>
       <c r="L15" t="s">
+        <v>72</v>
+      </c>
+      <c r="M15" t="s">
         <v>33</v>
-      </c>
-      <c r="M15">
-        <v>2</v>
       </c>
       <c r="N15">
         <v>2</v>
       </c>
       <c r="O15">
-        <v>1</v>
-      </c>
-      <c r="P15">
-        <v>1</v>
-      </c>
-      <c r="Q15" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="R15" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B16" t="s">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A16" s="4" t="s">
         <v>44</v>
       </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
       <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
-      <c r="E16">
+      <c r="F16">
         <v>42</v>
       </c>
-      <c r="F16">
+      <c r="G16">
         <v>435</v>
       </c>
-      <c r="H16">
+      <c r="I16">
         <f t="shared" si="1"/>
         <v>435</v>
       </c>
-      <c r="I16" s="2">
+      <c r="J16" s="2">
         <f t="shared" si="2"/>
         <v>10.357142857142858</v>
       </c>
-      <c r="J16" s="2">
-        <f t="shared" si="3"/>
-        <v>11.30952380952381</v>
-      </c>
-      <c r="K16" t="s">
+      <c r="K16" s="2">
+        <f t="shared" si="3"/>
+        <v>11.547619047619047</v>
+      </c>
+      <c r="L16" t="s">
         <v>42</v>
       </c>
-      <c r="L16" t="s">
+      <c r="M16" t="s">
         <v>33</v>
       </c>
-      <c r="M16">
-        <v>1</v>
-      </c>
       <c r="N16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O16">
         <v>0</v>
       </c>
-      <c r="P16">
-        <v>0</v>
-      </c>
-      <c r="Q16" s="1" t="s">
+      <c r="P16" t="s">
+        <v>74</v>
+      </c>
+      <c r="R16" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B17" t="s">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A17" s="4" t="s">
         <v>46</v>
       </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
       <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
-      <c r="D17">
+      <c r="E17">
         <v>52</v>
       </c>
-      <c r="E17">
+      <c r="F17">
         <v>46</v>
       </c>
-      <c r="F17">
+      <c r="G17">
         <v>450</v>
       </c>
-      <c r="G17">
+      <c r="H17">
         <v>50</v>
       </c>
-      <c r="H17">
+      <c r="I17">
         <f t="shared" si="1"/>
         <v>500</v>
       </c>
-      <c r="I17" s="2">
+      <c r="J17" s="2">
         <f t="shared" si="2"/>
         <v>10.869565217391305</v>
       </c>
-      <c r="J17" s="2">
+      <c r="K17" s="2">
         <f t="shared" si="3"/>
         <v>10.869565217391305</v>
       </c>
-      <c r="K17" t="s">
+      <c r="L17" t="s">
         <v>45</v>
       </c>
-      <c r="L17" t="s">
+      <c r="M17" t="s">
         <v>33</v>
       </c>
-      <c r="M17">
-        <v>1</v>
-      </c>
       <c r="N17">
         <v>1</v>
       </c>
@@ -1563,217 +1692,550 @@
       <c r="P17">
         <v>1</v>
       </c>
-      <c r="Q17" s="1" t="s">
+      <c r="R17" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B18" t="s">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A18" s="4" t="s">
         <v>48</v>
       </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
       <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="D18">
+      <c r="E18">
         <v>45</v>
       </c>
-      <c r="E18">
+      <c r="F18">
         <v>40</v>
       </c>
-      <c r="F18">
+      <c r="G18">
         <v>420</v>
       </c>
-      <c r="G18">
+      <c r="H18">
         <v>68</v>
       </c>
-      <c r="H18">
+      <c r="I18">
         <f t="shared" si="1"/>
         <v>488</v>
       </c>
-      <c r="I18" s="2">
+      <c r="J18" s="2">
         <f t="shared" si="2"/>
         <v>12.2</v>
       </c>
-      <c r="J18" s="2">
-        <f t="shared" si="3"/>
-        <v>13.2</v>
-      </c>
-      <c r="L18" t="s">
+      <c r="K18" s="2">
+        <f t="shared" si="3"/>
+        <v>13.45</v>
+      </c>
+      <c r="M18" t="s">
         <v>33</v>
       </c>
-      <c r="M18">
-        <v>1</v>
-      </c>
       <c r="N18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O18">
-        <v>0</v>
-      </c>
-      <c r="P18">
-        <v>1</v>
-      </c>
-      <c r="Q18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q18">
+        <v>1</v>
+      </c>
+      <c r="R18" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B19" t="s">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A19" s="4" t="s">
         <v>52</v>
       </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
       <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
-      <c r="D19">
+      <c r="E19">
         <v>50</v>
       </c>
-      <c r="E19">
+      <c r="F19">
         <v>45</v>
       </c>
-      <c r="F19">
+      <c r="G19">
         <v>400</v>
       </c>
-      <c r="G19">
+      <c r="H19">
         <v>120</v>
       </c>
-      <c r="H19">
+      <c r="I19">
         <f t="shared" si="1"/>
         <v>520</v>
       </c>
-      <c r="I19" s="2">
+      <c r="J19" s="2">
         <f t="shared" si="2"/>
         <v>11.555555555555555</v>
       </c>
-      <c r="J19" s="2">
-        <f t="shared" si="3"/>
-        <v>12.444444444444445</v>
-      </c>
-      <c r="K19" t="s">
+      <c r="K19" s="2">
+        <f t="shared" si="3"/>
+        <v>12.666666666666666</v>
+      </c>
+      <c r="L19" t="s">
         <v>53</v>
       </c>
-      <c r="L19" t="s">
+      <c r="M19" t="s">
         <v>33</v>
       </c>
-      <c r="M19">
-        <v>1</v>
-      </c>
       <c r="N19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O19">
         <v>0</v>
       </c>
-      <c r="P19">
-        <v>0</v>
-      </c>
-      <c r="Q19" s="1" t="s">
+      <c r="R19" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="20" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B20" t="s">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A20" s="4" t="s">
         <v>56</v>
       </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
       <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
         <f t="shared" si="0"/>
         <v>43</v>
       </c>
-      <c r="D20">
+      <c r="E20">
         <v>48</v>
       </c>
-      <c r="E20">
+      <c r="F20">
         <v>43</v>
       </c>
-      <c r="F20">
+      <c r="G20">
         <v>420</v>
       </c>
-      <c r="G20">
+      <c r="H20">
         <v>75</v>
       </c>
-      <c r="H20">
+      <c r="I20">
         <f t="shared" si="1"/>
         <v>495</v>
       </c>
-      <c r="I20" s="2">
+      <c r="J20" s="2">
         <f t="shared" si="2"/>
         <v>11.511627906976743</v>
       </c>
-      <c r="J20" s="2">
+      <c r="K20" s="2">
         <f t="shared" si="3"/>
         <v>11.511627906976743</v>
       </c>
-      <c r="L20" t="s">
+      <c r="M20" t="s">
         <v>33</v>
       </c>
-      <c r="M20">
-        <v>1</v>
-      </c>
       <c r="N20">
         <v>1</v>
       </c>
       <c r="O20">
         <v>1</v>
       </c>
-      <c r="P20">
-        <v>1</v>
-      </c>
-      <c r="Q20" s="1" t="s">
+      <c r="Q20">
+        <v>1</v>
+      </c>
+      <c r="R20" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B21" t="s">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A21" s="4" t="s">
         <v>59</v>
       </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
       <c r="C21">
-        <f t="shared" si="0"/>
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="D21">
+        <f t="shared" si="0"/>
         <v>50</v>
       </c>
       <c r="E21">
         <v>50</v>
       </c>
       <c r="F21">
+        <v>50</v>
+      </c>
+      <c r="G21">
         <v>360</v>
       </c>
-      <c r="G21">
+      <c r="H21">
         <v>80</v>
       </c>
-      <c r="H21">
+      <c r="I21">
         <f t="shared" si="1"/>
         <v>440</v>
       </c>
-      <c r="I21" s="2">
+      <c r="J21" s="2">
         <f t="shared" si="2"/>
         <v>8.8000000000000007</v>
       </c>
-      <c r="J21" s="2">
-        <f t="shared" si="3"/>
-        <v>9.6</v>
-      </c>
-      <c r="L21" t="s">
+      <c r="K21" s="2">
+        <f t="shared" si="3"/>
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="M21" t="s">
         <v>33</v>
       </c>
-      <c r="M21">
-        <v>1</v>
-      </c>
       <c r="N21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O21">
-        <v>0</v>
-      </c>
-      <c r="P21">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="R21" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A22" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="E22">
+        <v>48</v>
+      </c>
+      <c r="F22">
+        <v>48</v>
+      </c>
+      <c r="G22">
+        <v>430</v>
+      </c>
+      <c r="H22">
+        <v>90</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="1"/>
+        <v>520</v>
+      </c>
+      <c r="J22" s="2">
+        <f t="shared" si="2"/>
+        <v>10.833333333333334</v>
+      </c>
+      <c r="K22" s="2">
+        <f t="shared" si="3"/>
+        <v>10.833333333333334</v>
+      </c>
+      <c r="M22" t="s">
+        <v>33</v>
+      </c>
+      <c r="N22">
+        <v>1</v>
+      </c>
+      <c r="O22">
+        <v>1</v>
+      </c>
+      <c r="Q22">
+        <v>1</v>
+      </c>
+      <c r="R22" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A23" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="E23">
+        <v>45</v>
+      </c>
+      <c r="F23">
+        <v>42</v>
+      </c>
+      <c r="G23">
+        <v>450</v>
+      </c>
+      <c r="H23">
+        <v>75</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="1"/>
+        <v>525</v>
+      </c>
+      <c r="J23" s="2">
+        <f t="shared" si="2"/>
+        <v>12.5</v>
+      </c>
+      <c r="K23" s="2">
+        <f t="shared" si="3"/>
+        <v>12.5</v>
+      </c>
+      <c r="M23" t="s">
+        <v>33</v>
+      </c>
+      <c r="N23">
+        <v>1</v>
+      </c>
+      <c r="O23">
+        <v>1</v>
+      </c>
+      <c r="Q23">
+        <v>1</v>
+      </c>
+      <c r="R23" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A24" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="E24">
+        <v>57</v>
+      </c>
+      <c r="F24">
+        <v>45</v>
+      </c>
+      <c r="G24">
+        <v>450</v>
+      </c>
+      <c r="H24">
+        <v>100</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="1"/>
+        <v>550</v>
+      </c>
+      <c r="J24" s="2">
+        <f t="shared" si="2"/>
+        <v>12.222222222222221</v>
+      </c>
+      <c r="K24" s="2">
+        <f t="shared" si="3"/>
+        <v>13.333333333333334</v>
+      </c>
+      <c r="M24" t="s">
+        <v>33</v>
+      </c>
+      <c r="N24">
+        <v>0</v>
+      </c>
+      <c r="O24">
+        <v>1</v>
+      </c>
+      <c r="Q24">
+        <v>1</v>
+      </c>
+      <c r="R24" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A25" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="E25">
+        <v>40</v>
+      </c>
+      <c r="F25">
+        <v>40</v>
+      </c>
+      <c r="G25">
+        <v>380</v>
+      </c>
+      <c r="H25">
+        <v>75</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="1"/>
+        <v>455</v>
+      </c>
+      <c r="J25" s="2">
+        <f t="shared" si="2"/>
+        <v>11.375</v>
+      </c>
+      <c r="K25" s="2">
+        <f t="shared" si="3"/>
+        <v>11.375</v>
+      </c>
+      <c r="M25" t="s">
+        <v>33</v>
+      </c>
+      <c r="N25">
+        <v>1</v>
+      </c>
+      <c r="O25">
+        <v>1</v>
+      </c>
+      <c r="R25" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A26" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="E26">
+        <v>50</v>
+      </c>
+      <c r="F26">
+        <v>50</v>
+      </c>
+      <c r="G26">
+        <v>400</v>
+      </c>
+      <c r="H26">
+        <v>100</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="1"/>
+        <v>500</v>
+      </c>
+      <c r="J26" s="2">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="K26" s="2">
+        <f t="shared" si="3"/>
+        <v>11</v>
+      </c>
+      <c r="M26" t="s">
+        <v>33</v>
+      </c>
+      <c r="N26">
+        <v>0</v>
+      </c>
+      <c r="O26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>56</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="E27">
+        <v>57</v>
+      </c>
+      <c r="F27">
+        <v>45</v>
+      </c>
+      <c r="G27">
+        <v>400</v>
+      </c>
+      <c r="H27">
+        <v>120</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="1"/>
+        <v>520</v>
+      </c>
+      <c r="J27" s="2">
+        <f t="shared" si="2"/>
+        <v>11.555555555555555</v>
+      </c>
+      <c r="K27" s="2">
+        <f t="shared" si="3"/>
+        <v>11.555555555555555</v>
+      </c>
+      <c r="M27" t="s">
+        <v>33</v>
+      </c>
+      <c r="N27">
+        <v>1</v>
+      </c>
+      <c r="O27">
+        <v>1</v>
+      </c>
+      <c r="R27" s="1" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="J2:J21">
-    <cfRule type="colorScale" priority="1">
+  <conditionalFormatting sqref="K2:K27">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I2:I27">
+    <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1785,27 +2247,34 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="Q2" r:id="rId1" xr:uid="{BC09F7C9-7B72-4359-95B0-C2E1E05EF957}"/>
-    <hyperlink ref="Q3" r:id="rId2" xr:uid="{F038CDB1-8A86-4688-A6D6-EFF4B88ACBC9}"/>
-    <hyperlink ref="Q4" r:id="rId3" xr:uid="{DA72C175-A4E0-46ED-9774-B5F9A8BBBAE0}"/>
-    <hyperlink ref="Q5" r:id="rId4" xr:uid="{FE2AA06A-6A35-4937-BE49-B7B45B21F0D5}"/>
-    <hyperlink ref="Q6" r:id="rId5" xr:uid="{2E4012BE-EB79-4012-A169-A991ACE7F117}"/>
-    <hyperlink ref="Q7" r:id="rId6" xr:uid="{A02D9B5E-53BF-4A4A-BDC2-FE594C51D634}"/>
-    <hyperlink ref="Q8" r:id="rId7" xr:uid="{8FA9A79E-6898-4660-9DE9-6F7EFEA61F05}"/>
-    <hyperlink ref="Q9" r:id="rId8" xr:uid="{B88818F4-85EA-4C04-A015-0ECD67F9BC0C}"/>
-    <hyperlink ref="Q10" r:id="rId9" xr:uid="{12FE4701-FD57-4DEE-A050-02AA65B15321}"/>
-    <hyperlink ref="Q12" r:id="rId10" xr:uid="{8D75F53D-2337-467A-B53E-FC3A975384F5}"/>
-    <hyperlink ref="Q14" r:id="rId11" xr:uid="{E55BA592-81C1-4CFF-B914-814C72CD5900}"/>
-    <hyperlink ref="Q13" r:id="rId12" xr:uid="{CC2D0F41-FC4B-4FBE-BA19-4A2F07D1C48B}"/>
-    <hyperlink ref="Q15" r:id="rId13" xr:uid="{F01F7903-CB22-4162-976E-157168585DF5}"/>
-    <hyperlink ref="Q16" r:id="rId14" location="lofts" xr:uid="{7C02D451-FEA2-4D9B-A8CC-2BB27509D8FF}"/>
-    <hyperlink ref="Q17" r:id="rId15" xr:uid="{D8C6B8A0-C8A3-4B20-82FD-064CF0E61167}"/>
-    <hyperlink ref="Q18" r:id="rId16" xr:uid="{C8851664-C1E9-4EFC-B52A-BDC05728D40F}"/>
-    <hyperlink ref="Q19" r:id="rId17" xr:uid="{D5C3517C-A7D7-4944-8840-1CF35728AA10}"/>
-    <hyperlink ref="Q20" r:id="rId18" xr:uid="{8F083F3D-C61C-4983-BE1E-3B788A7C8D12}"/>
+    <hyperlink ref="R2" r:id="rId1" xr:uid="{BC09F7C9-7B72-4359-95B0-C2E1E05EF957}"/>
+    <hyperlink ref="R3" r:id="rId2" xr:uid="{F038CDB1-8A86-4688-A6D6-EFF4B88ACBC9}"/>
+    <hyperlink ref="R4" r:id="rId3" xr:uid="{DA72C175-A4E0-46ED-9774-B5F9A8BBBAE0}"/>
+    <hyperlink ref="R5" r:id="rId4" xr:uid="{FE2AA06A-6A35-4937-BE49-B7B45B21F0D5}"/>
+    <hyperlink ref="R6" r:id="rId5" xr:uid="{2E4012BE-EB79-4012-A169-A991ACE7F117}"/>
+    <hyperlink ref="R7" r:id="rId6" xr:uid="{A02D9B5E-53BF-4A4A-BDC2-FE594C51D634}"/>
+    <hyperlink ref="R8" r:id="rId7" xr:uid="{8FA9A79E-6898-4660-9DE9-6F7EFEA61F05}"/>
+    <hyperlink ref="R9" r:id="rId8" xr:uid="{B88818F4-85EA-4C04-A015-0ECD67F9BC0C}"/>
+    <hyperlink ref="R10" r:id="rId9" xr:uid="{12FE4701-FD57-4DEE-A050-02AA65B15321}"/>
+    <hyperlink ref="R12" r:id="rId10" xr:uid="{8D75F53D-2337-467A-B53E-FC3A975384F5}"/>
+    <hyperlink ref="R14" r:id="rId11" xr:uid="{E55BA592-81C1-4CFF-B914-814C72CD5900}"/>
+    <hyperlink ref="R13" r:id="rId12" xr:uid="{CC2D0F41-FC4B-4FBE-BA19-4A2F07D1C48B}"/>
+    <hyperlink ref="R15" r:id="rId13" xr:uid="{F01F7903-CB22-4162-976E-157168585DF5}"/>
+    <hyperlink ref="R16" r:id="rId14" location="lofts" xr:uid="{7C02D451-FEA2-4D9B-A8CC-2BB27509D8FF}"/>
+    <hyperlink ref="R17" r:id="rId15" xr:uid="{D8C6B8A0-C8A3-4B20-82FD-064CF0E61167}"/>
+    <hyperlink ref="R18" r:id="rId16" xr:uid="{C8851664-C1E9-4EFC-B52A-BDC05728D40F}"/>
+    <hyperlink ref="R19" r:id="rId17" xr:uid="{D5C3517C-A7D7-4944-8840-1CF35728AA10}"/>
+    <hyperlink ref="R20" r:id="rId18" xr:uid="{8F083F3D-C61C-4983-BE1E-3B788A7C8D12}"/>
+    <hyperlink ref="R22" r:id="rId19" location="reco_item_pos=14&amp;reco_backend=user_navigation&amp;reco_backend_type=function&amp;reco_client=classi_portalinmobiliario_navigation&amp;reco_id=ae77e213-7c53-4a83-8240-0ef49e221d10&amp;page=navigation" display="https://www.portalinmobiliario.com/MLC-545543913-departamento-en-arriendo-de-1-dorm-en-providencia-_JM#reco_item_pos=14&amp;reco_backend=user_navigation&amp;reco_backend_type=function&amp;reco_client=classi_portalinmobiliario_navigation&amp;reco_id=ae77e213-7c53-4a83-8240-0ef49e221d10&amp;page=navigation" xr:uid="{54D87716-23AE-4CC3-9D9E-286844F50FE0}"/>
+    <hyperlink ref="R23" r:id="rId20" xr:uid="{729A05BC-26F7-4A89-96EC-A11EC91C2059}"/>
+    <hyperlink ref="R24" r:id="rId21" xr:uid="{ECF044AF-C32F-4658-868C-7650EFAAD592}"/>
+    <hyperlink ref="R25" r:id="rId22" xr:uid="{B10E86EA-8BBE-4857-A06C-B23C1AE64687}"/>
+    <hyperlink ref="R27" r:id="rId23" xr:uid="{FDC3F1A5-2A3D-4FE5-9420-92CB1B59895B}"/>
+    <hyperlink ref="R11" r:id="rId24" xr:uid="{C12B89CE-D16B-48A2-8F2D-5AC24BC547EB}"/>
+    <hyperlink ref="R21" r:id="rId25" xr:uid="{7D76AFF2-23E1-48A7-B220-4ADEA18BA472}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId19"/>
-  <legacyDrawing r:id="rId20"/>
+  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId26"/>
+  <legacyDrawing r:id="rId27"/>
 </worksheet>
 </file>
</xml_diff>